<commit_message>
Updated readme and sample form based on updates to code
</commit_message>
<xml_diff>
--- a/extras/sample-form/Extra buttons.xlsx
+++ b/extras/sample-form/Extra buttons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Dobility support/Field plug-ins/Plug-ins by Max/In progress/extra-buttons/extras/sample-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C692083-C62C-DD43-8EFB-D60ADFC244DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBB2798-AAE3-064D-83D6-EDC08EC6104D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="900" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26360" yWindow="460" windowWidth="25000" windowHeight="15540" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2668,13 +2668,13 @@
     <t>custom-extrabuttons(button1="I don't know", value1=-99, button2="I don't understand the question", value2=-77, button3="Who are you? How did I get here?", value3=-66, button4="Qu'est-ce que vous avez dit?", value4=-55, no='Nope')</t>
   </si>
   <si>
-    <t>custom-extrabuttons(button1="I don't know", value1=-99, button2='Refused', value2=-88, button3="I don't understand the question", value3=-77, warning='Voulez-vous vraiment remplacer "oldValue" par "replacementValue"?', yes='Oui', no='Non')</t>
-  </si>
-  <si>
     <t>custom-extrabuttons(button1='Refused', value1=-88)</t>
   </si>
   <si>
-    <t>custom-extrabuttons(message='هل أنت متأكد من أنك تريد استبدال القيمة؟', yes='نعم', no='لا', button1='رفض', value1=-88)</t>
+    <t>custom-extrabuttons(button1="I don't know", value1=-99, button2='Refused', value2=-88, button3="I don't understand the question", value3=-77, warning='Attention: ce champ a déjà une valeur. Etes-vous sûr de vouloir le remplacer?', yes='Oui', no='Non')</t>
+  </si>
+  <si>
+    <t>custom-extrabuttons(warning='هل أنت متأكد من أنك تريد استبدال القيمة؟', yes='نعم', no='لا', button1='رفض', value1=-88)</t>
   </si>
 </sst>
 </file>
@@ -4835,7 +4835,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4845,7 +4845,7 @@
     <col min="3" max="3" width="30.5" style="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="23" style="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7.1640625" style="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.6640625" style="9" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="79" style="9" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17.1640625" style="9" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="17" style="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="17.33203125" style="9" customWidth="1" collapsed="1"/>
@@ -5177,7 +5177,7 @@
         <v>385</v>
       </c>
       <c r="F12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G12" t="s">
         <v>358</v>
@@ -5219,7 +5219,7 @@
         <v>385</v>
       </c>
       <c r="F13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G13" t="s">
         <v>387</v>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2005182138</v>
+        <v>2009160021</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>

</xml_diff>